<commit_message>
add one more time estimate
</commit_message>
<xml_diff>
--- a/subproblem breakup.xlsx
+++ b/subproblem breakup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/abce12e681c5cf45/research/repro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avi\OneDrive\research\repro\Crime-and-Climate-Change-Reproduction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{E9A57E51-5E75-4941-9DD7-0C9BFCFA1D87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{2D9844DB-AF15-4CF1-AEC5-C0CC9787F8AC}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{E9A57E51-5E75-4941-9DD7-0C9BFCFA1D87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{93B5241C-C797-4897-ADD4-701651C0805D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12900" windowHeight="8888" xr2:uid="{79792660-E7BA-4F86-A522-05C82B40E397}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>subproblem</t>
   </si>
@@ -87,9 +87,6 @@
     <t>laptop time</t>
   </si>
   <si>
-    <t>9:38 (using most naïve algorithm; can definitely be improved by only looking at stations from neighboring states)</t>
-  </si>
-  <si>
     <t>link to stations dataframe can be provided</t>
   </si>
   <si>
@@ -190,6 +187,12 @@
   </si>
   <si>
     <t>generate regression coefficients</t>
+  </si>
+  <si>
+    <t>~5:00</t>
+  </si>
+  <si>
+    <t>~10:00 (using most naïve algorithm; can definitely be improved by only looking at stations from neighboring states)</t>
   </si>
 </sst>
 </file>
@@ -557,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF97471-496F-4CAE-AE07-1BB84A30E34F}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -641,7 +644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -649,10 +652,10 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
@@ -663,62 +666,65 @@
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
+      <c r="D13" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
@@ -726,90 +732,90 @@
     </row>
     <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>